<commit_message>
Models and Migrations and Views, Paginate, View Details List
</commit_message>
<xml_diff>
--- a/storage/archivos/importar_vuelos.xlsx
+++ b/storage/archivos/importar_vuelos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>hora_despegue</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Nueva York</t>
+  </si>
+  <si>
+    <t>costo</t>
   </si>
 </sst>
 </file>
@@ -124,11 +127,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,15 +447,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -485,16 +492,19 @@
       <c r="K1" t="s">
         <v>15</v>
       </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1">
-        <v>0.29166666666666669</v>
+      <c r="C2" s="4">
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -520,8 +530,11 @@
       <c r="K2" t="s">
         <v>16</v>
       </c>
+      <c r="L2">
+        <v>1200</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
     </row>
   </sheetData>

</xml_diff>